<commit_message>
add vài cái test
</commit_message>
<xml_diff>
--- a/Bai1/testcase.xlsx
+++ b/Bai1/testcase.xlsx
@@ -2758,6 +2758,158 @@
         <a:xfrm>
           <a:off x="8696739" y="24152087"/>
           <a:ext cx="2335696" cy="2857500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>57979</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>704023</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1739348" y="28848327"/>
+          <a:ext cx="2377109" cy="704022"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>712305</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>66261</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1341784</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1739348" y="29560631"/>
+          <a:ext cx="2385391" cy="629479"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>8283</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1424609</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>41413</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>2100978</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1747631" y="30272935"/>
+          <a:ext cx="2352260" cy="676369"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>66262</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>8283</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>82827</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1027044</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4124740" y="28856609"/>
+          <a:ext cx="2335696" cy="1018761"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3069,7 +3221,7 @@
   <dimension ref="A1:V18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:G15"/>
+      <selection activeCell="A15" sqref="A15:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="69.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3433,7 +3585,7 @@
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
     </row>
-    <row r="15" spans="1:22" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
@@ -3535,80 +3687,16 @@
     </row>
   </sheetData>
   <mergeCells count="108">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="L5:O5"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="L7:O7"/>
-    <mergeCell ref="L8:O8"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="L13:O13"/>
-    <mergeCell ref="L9:O9"/>
-    <mergeCell ref="L10:O10"/>
-    <mergeCell ref="L11:O11"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="P6:R6"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="S6:U6"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="P7:R7"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="P12:R12"/>
-    <mergeCell ref="S13:U13"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="S9:U9"/>
-    <mergeCell ref="S10:U10"/>
-    <mergeCell ref="S11:U11"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="L3:O3"/>
-    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S17:U17"/>
+    <mergeCell ref="S18:U18"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="S14:U14"/>
+    <mergeCell ref="S15:U15"/>
+    <mergeCell ref="S16:U16"/>
+    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="P15:R15"/>
     <mergeCell ref="S3:U3"/>
     <mergeCell ref="S12:U12"/>
     <mergeCell ref="L12:O12"/>
@@ -3633,16 +3721,80 @@
     <mergeCell ref="L16:O16"/>
     <mergeCell ref="L17:O17"/>
     <mergeCell ref="L18:O18"/>
-    <mergeCell ref="S17:U17"/>
-    <mergeCell ref="S18:U18"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="S14:U14"/>
-    <mergeCell ref="S15:U15"/>
-    <mergeCell ref="S16:U16"/>
-    <mergeCell ref="P14:R14"/>
-    <mergeCell ref="P15:R15"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="P10:R10"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="P12:R12"/>
+    <mergeCell ref="S13:U13"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="S9:U9"/>
+    <mergeCell ref="S10:U10"/>
+    <mergeCell ref="S11:U11"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="L8:O8"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="L13:O13"/>
+    <mergeCell ref="L9:O9"/>
+    <mergeCell ref="L10:O10"/>
+    <mergeCell ref="L11:O11"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="L5:O5"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
fix lựa chọn 8 (lỗi do import datetime cách khác)
</commit_message>
<xml_diff>
--- a/Bai1/testcase.xlsx
+++ b/Bai1/testcase.xlsx
@@ -2883,33 +2883,337 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>66262</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>14</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>8282</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>770283</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Picture 40"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4058478" y="28848327"/>
+          <a:ext cx="2327413" cy="770282"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>41413</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>770282</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>579782</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1805609</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="Picture 43"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4099891" y="29618608"/>
+          <a:ext cx="2277717" cy="1035327"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>49696</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1797326</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>49695</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>2700132</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Picture 44"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4108174" y="30645652"/>
+          <a:ext cx="2319130" cy="902806"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>16565</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>2799522</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>41413</xdr:colOff>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>8283</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="51" name="Picture 50"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4075043" y="31647848"/>
+          <a:ext cx="2343979" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>82827</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>1027044</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="Picture 25"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4124740" y="28856609"/>
-          <a:ext cx="2335696" cy="1018761"/>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>563217</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1085022</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="55" name="Picture 54"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6377609" y="28848326"/>
+          <a:ext cx="2302565" cy="1085022"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>563217</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1085022</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="92" name="Picture 91"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8696739" y="28848326"/>
+          <a:ext cx="2302565" cy="1085022"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>24848</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>381000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="93" name="Picture 92"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4058478" y="32020565"/>
+          <a:ext cx="2343979" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>563217</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1085022</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="95" name="Picture 94"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6377609" y="32020565"/>
+          <a:ext cx="2302565" cy="1085022"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>563217</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1085022</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="96" name="Picture 95"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8696739" y="32020565"/>
+          <a:ext cx="2302565" cy="1085022"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3220,8 +3524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:C15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16:R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="69.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3585,7 +3889,7 @@
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
     </row>
-    <row r="15" spans="1:22" ht="180" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="249.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
@@ -3687,16 +3991,80 @@
     </row>
   </sheetData>
   <mergeCells count="108">
-    <mergeCell ref="S17:U17"/>
-    <mergeCell ref="S18:U18"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="S14:U14"/>
-    <mergeCell ref="S15:U15"/>
-    <mergeCell ref="S16:U16"/>
-    <mergeCell ref="P14:R14"/>
-    <mergeCell ref="P15:R15"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="L5:O5"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="L8:O8"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="L13:O13"/>
+    <mergeCell ref="L9:O9"/>
+    <mergeCell ref="L10:O10"/>
+    <mergeCell ref="L11:O11"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="P10:R10"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="P12:R12"/>
+    <mergeCell ref="S13:U13"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="S9:U9"/>
+    <mergeCell ref="S10:U10"/>
+    <mergeCell ref="S11:U11"/>
+    <mergeCell ref="P3:R3"/>
     <mergeCell ref="S3:U3"/>
     <mergeCell ref="S12:U12"/>
     <mergeCell ref="L12:O12"/>
@@ -3721,80 +4089,16 @@
     <mergeCell ref="L16:O16"/>
     <mergeCell ref="L17:O17"/>
     <mergeCell ref="L18:O18"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="P6:R6"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="S6:U6"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="P7:R7"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="P12:R12"/>
-    <mergeCell ref="S13:U13"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="S9:U9"/>
-    <mergeCell ref="S10:U10"/>
-    <mergeCell ref="S11:U11"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="L7:O7"/>
-    <mergeCell ref="L8:O8"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="L13:O13"/>
-    <mergeCell ref="L9:O9"/>
-    <mergeCell ref="L10:O10"/>
-    <mergeCell ref="L11:O11"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="L5:O5"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="S17:U17"/>
+    <mergeCell ref="S18:U18"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="S14:U14"/>
+    <mergeCell ref="S15:U15"/>
+    <mergeCell ref="S16:U16"/>
+    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="P15:R15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Code chạy nuột rồi
</commit_message>
<xml_diff>
--- a/Bai1/testcase.xlsx
+++ b/Bai1/testcase.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tensorflow\Documents\UDKT\Bai1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LAPTRINUDCHOKT\pythonProject\BTL\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652636C7-E68B-4366-85E1-F0749E267C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Tên test case</t>
   </si>
@@ -77,9 +78,6 @@
     <t>Thêm một số lượng phương tiện vào bãi đậu xe và thiết lập một số xe có nhiều lượt gửi trong ngày</t>
   </si>
   <si>
-    <t>Kiểm tra xem danh sách xe có nhiều lượt gửi trong ngày hiện tại đã hiển thị đúng</t>
-  </si>
-  <si>
     <t>Xóa xe đang đỗ thành công với thông tin hợp lệ</t>
   </si>
   <si>
@@ -91,12 +89,18 @@
   <si>
     <t>Nhập loại xe lỗi</t>
   </si>
+  <si>
+    <t>Kiểm tra xem danh sách xe có nhiều lượt gửi trong ngày hiện tại đã hiển thị đúng ( không tính xe ngày hôm qua)</t>
+  </si>
+  <si>
+    <t>dữ liệu có sẵn : có xe hôm qua , xe sáng , xe tối . B1 lấy xe sáng ( tối ) , hôm qua . B2 thêm xe sáng (tối ) , hôm qua . B3 chọn 8 để xem danh sách xe gửi từ 2 lần trở lên ( có thể chọn 9 để kiêmtra kết quả ) -&gt; kết quả xe sáng (tối ) 2 lần , xe hôm qua tuy xuất hiện 2 lần ( danh sách choice "9"  nhưng nó là 2 ngày.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,7 +172,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -199,14 +209,20 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>563216</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1159564</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>24848</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -238,13 +254,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>546653</xdr:colOff>
+      <xdr:colOff>115957</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>33132</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -275,14 +297,20 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>430697</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1027046</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>33131</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -320,7 +348,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -351,14 +385,20 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>521803</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1118151</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>37815</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -390,13 +430,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>546653</xdr:colOff>
+      <xdr:colOff>115957</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>41413</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -427,14 +473,20 @@
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>422413</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1018762</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>41414</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9"/>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -472,7 +524,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11"/>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -503,14 +561,20 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>505238</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1101586</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12"/>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -542,13 +606,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>521805</xdr:colOff>
+      <xdr:colOff>91109</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13"/>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -579,14 +649,20 @@
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>405849</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1002198</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>869675</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 14"/>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -624,7 +700,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Picture 15"/>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -655,14 +737,20 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>521804</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1118152</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>16565</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Picture 16"/>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -694,13 +782,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>546653</xdr:colOff>
+      <xdr:colOff>115957</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>33131</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Picture 17"/>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -731,14 +825,20 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>546652</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1739349</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>33130</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Picture 18"/>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -776,7 +876,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Picture 19"/>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -807,14 +913,20 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>513522</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1109870</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>902804</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Picture 20"/>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -846,13 +958,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>530087</xdr:colOff>
+      <xdr:colOff>99391</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>2505425</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="Picture 21"/>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -883,14 +1001,20 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>530086</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1722783</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>2505425</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Picture 22"/>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -928,7 +1052,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="Picture 23"/>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -966,7 +1096,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="27" name="Picture 26"/>
+        <xdr:cNvPr id="27" name="Picture 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1004,7 +1140,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="Picture 27"/>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1037,7 +1179,13 @@
     <xdr:ext cx="2865783" cy="590632"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="29" name="Picture 28"/>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1070,7 +1218,13 @@
     <xdr:ext cx="2849218" cy="562053"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="Picture 29"/>
+        <xdr:cNvPr id="30" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1103,7 +1257,13 @@
     <xdr:ext cx="2857501" cy="666843"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="31" name="Picture 30"/>
+        <xdr:cNvPr id="31" name="Picture 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1135,13 +1295,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>530087</xdr:colOff>
+      <xdr:colOff>99391</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>8284</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="32" name="Picture 31"/>
+        <xdr:cNvPr id="32" name="Picture 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1172,14 +1338,20 @@
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>530086</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1722783</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>33132</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="33" name="Picture 32"/>
+        <xdr:cNvPr id="33" name="Picture 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1211,13 +1383,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>554935</xdr:colOff>
+      <xdr:colOff>124239</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>902805</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="34" name="Picture 33"/>
+        <xdr:cNvPr id="34" name="Picture 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1248,14 +1426,20 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>554935</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1747632</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>911087</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="35" name="Picture 34"/>
+        <xdr:cNvPr id="35" name="Picture 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1293,7 +1477,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="36" name="Picture 35"/>
+        <xdr:cNvPr id="36" name="Picture 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1324,14 +1514,20 @@
       <xdr:rowOff>2236304</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>554934</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1151282</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>3130826</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="37" name="Picture 36"/>
+        <xdr:cNvPr id="37" name="Picture 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1364,7 +1560,13 @@
     <xdr:ext cx="2302565" cy="590632"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="38" name="Picture 37"/>
+        <xdr:cNvPr id="38" name="Picture 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1397,7 +1599,13 @@
     <xdr:ext cx="2310848" cy="562053"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="39" name="Picture 38"/>
+        <xdr:cNvPr id="39" name="Picture 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1430,7 +1638,13 @@
     <xdr:ext cx="2335696" cy="666843"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="40" name="Picture 39"/>
+        <xdr:cNvPr id="40" name="Picture 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1468,7 +1682,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="46" name="Picture 45"/>
+        <xdr:cNvPr id="46" name="Picture 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1501,7 +1721,13 @@
     <xdr:ext cx="2816087" cy="590632"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="47" name="Picture 46"/>
+        <xdr:cNvPr id="47" name="Picture 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1534,7 +1760,13 @@
     <xdr:ext cx="2849218" cy="562053"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="48" name="Picture 47"/>
+        <xdr:cNvPr id="48" name="Picture 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1567,7 +1799,13 @@
     <xdr:ext cx="2857501" cy="666843"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="49" name="Picture 48"/>
+        <xdr:cNvPr id="49" name="Picture 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1600,7 +1838,13 @@
     <xdr:ext cx="2874065" cy="894522"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="50" name="Picture 49"/>
+        <xdr:cNvPr id="50" name="Picture 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000032000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1631,14 +1875,20 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>538369</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1134717</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>657317</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="52" name="Picture 51"/>
+        <xdr:cNvPr id="52" name="Picture 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000034000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1670,13 +1920,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>530087</xdr:colOff>
+      <xdr:colOff>99391</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>4944718</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="53" name="Picture 52"/>
+        <xdr:cNvPr id="53" name="Picture 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000035000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1707,14 +1963,20 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>530086</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1722783</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>4953000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="54" name="Picture 53"/>
+        <xdr:cNvPr id="54" name="Picture 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000036000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1745,14 +2007,20 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>538369</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1134717</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>400106</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="63" name="Picture 62"/>
+        <xdr:cNvPr id="63" name="Picture 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1784,13 +2052,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>546653</xdr:colOff>
+      <xdr:colOff>115957</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>438980</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="64" name="Picture 63"/>
+        <xdr:cNvPr id="64" name="Picture 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000040000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1821,14 +2095,20 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>414131</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1010480</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>472109</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="65" name="Picture 64"/>
+        <xdr:cNvPr id="65" name="Picture 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000041000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1861,7 +2141,13 @@
     <xdr:ext cx="2277717" cy="590632"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="66" name="Picture 65"/>
+        <xdr:cNvPr id="66" name="Picture 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000042000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1894,7 +2180,13 @@
     <xdr:ext cx="2277719" cy="562053"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="67" name="Picture 66"/>
+        <xdr:cNvPr id="67" name="Picture 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000043000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1927,7 +2219,13 @@
     <xdr:ext cx="2302566" cy="455544"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="68" name="Picture 67"/>
+        <xdr:cNvPr id="68" name="Picture 67">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000044000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1960,7 +2258,13 @@
     <xdr:ext cx="2277716" cy="646043"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="69" name="Picture 68"/>
+        <xdr:cNvPr id="69" name="Picture 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000045000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1991,14 +2295,20 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>596348</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>562053</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="70" name="Picture 69"/>
+        <xdr:cNvPr id="70" name="Picture 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000046000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2030,13 +2340,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>554934</xdr:colOff>
+      <xdr:colOff>554935</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>1057423</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="71" name="Picture 70"/>
+        <xdr:cNvPr id="71" name="Picture 70">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000047000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2067,14 +2383,20 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>554934</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1151283</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>1057423</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="72" name="Picture 71"/>
+        <xdr:cNvPr id="72" name="Picture 71">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000048000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2112,7 +2434,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="73" name="Picture 72"/>
+        <xdr:cNvPr id="73" name="Picture 72">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000049000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2143,14 +2471,20 @@
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>16565</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>612913</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>869675</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="75" name="Picture 74"/>
+        <xdr:cNvPr id="75" name="Picture 74">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2181,14 +2515,20 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>596350</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>877957</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="76" name="Picture 75"/>
+        <xdr:cNvPr id="76" name="Picture 75">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2226,7 +2566,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="77" name="Picture 76"/>
+        <xdr:cNvPr id="77" name="Picture 76">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2249,219 +2595,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>16566</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>16565</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>861391</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="78" name="Picture 77"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4075044" y="31258565"/>
-          <a:ext cx="2294282" cy="844826"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>521804</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>861391</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="79" name="Picture 78"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6377609" y="31242000"/>
-          <a:ext cx="2261152" cy="861391"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>521804</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>861391</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="80" name="Picture 79"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8696739" y="31242000"/>
-          <a:ext cx="2261152" cy="861391"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>16565</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>8283</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2302565" cy="590632"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="81" name="Picture 80"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1755913" y="11603935"/>
-          <a:ext cx="2302565" cy="590632"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>670891</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2310848" cy="562053"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="82" name="Picture 81"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1739348" y="12266543"/>
-          <a:ext cx="2310848" cy="562053"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>563217</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>1399761</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2335696" cy="666843"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="83" name="Picture 82"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1722782" y="12995413"/>
-          <a:ext cx="2335696" cy="666843"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
@@ -2477,13 +2610,19 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="84" name="Picture 83"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <xdr:cNvPr id="84" name="Picture 83">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000054000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2508,20 +2647,26 @@
       <xdr:rowOff>2410238</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>24847</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>621195</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>803412</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="85" name="Picture 84"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <xdr:cNvPr id="85" name="Picture 84">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000055000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2553,13 +2698,19 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="86" name="Picture 85"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <xdr:cNvPr id="86" name="Picture 85">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000056000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2584,20 +2735,26 @@
       <xdr:rowOff>1764196</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>8282</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>604630</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>2658717</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="87" name="Picture 86"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+        <xdr:cNvPr id="87" name="Picture 86">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000057000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2617,33 +2774,39 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>16565</xdr:colOff>
+      <xdr:colOff>48991</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>2700130</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>546651</xdr:colOff>
+      <xdr:rowOff>2927108</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1505745</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>3743738</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="88" name="Picture 87"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4075043" y="26852217"/>
-          <a:ext cx="4588565" cy="1043608"/>
+      <xdr:rowOff>3647873</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="88" name="Picture 87">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000058000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4248097" y="27148980"/>
+          <a:ext cx="3256371" cy="720765"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2660,20 +2823,26 @@
       <xdr:rowOff>3810000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>8283</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>604631</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>4172001</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="89" name="Picture 88"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
+        <xdr:cNvPr id="89" name="Picture 88">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000059000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2699,19 +2868,25 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>530087</xdr:colOff>
+      <xdr:colOff>530088</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>2178326</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="90" name="Picture 89"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
+        <xdr:cNvPr id="90" name="Picture 89">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2736,20 +2911,26 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>16565</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1209262</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>2857500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="91" name="Picture 90"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
+        <xdr:cNvPr id="91" name="Picture 90">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2781,13 +2962,19 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2819,13 +3006,19 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2857,13 +3050,19 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="Picture 24"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
+        <xdr:cNvPr id="25" name="Picture 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2888,20 +3087,26 @@
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>8282</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>604630</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>770283</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="41" name="Picture 40"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
+        <xdr:cNvPr id="41" name="Picture 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2933,13 +3138,19 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="44" name="Picture 43"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
+        <xdr:cNvPr id="44" name="Picture 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2964,20 +3175,26 @@
       <xdr:rowOff>1797326</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>49695</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>646043</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>2700132</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="45" name="Picture 44"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42"/>
+        <xdr:cNvPr id="45" name="Picture 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3002,20 +3219,26 @@
       <xdr:rowOff>2799522</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>41413</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>637761</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>8283</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="51" name="Picture 50"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43"/>
+        <xdr:cNvPr id="51" name="Picture 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000033000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3041,19 +3264,25 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>563217</xdr:colOff>
+      <xdr:colOff>563218</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>1085022</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="55" name="Picture 54"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
+        <xdr:cNvPr id="55" name="Picture 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000037000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3078,20 +3307,26 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>563217</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1159566</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>1085022</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="92" name="Picture 91"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
+        <xdr:cNvPr id="92" name="Picture 91">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3110,34 +3345,348 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>132524</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>245165</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>568522</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1782417</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92F0ED12-8847-4F54-A669-F21C1EF7DF04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1921567" y="32222661"/>
+          <a:ext cx="2225042" cy="1537252"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>66260</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>510208</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>447512</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1457738</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="42" name="Picture 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1694D2A7-34FF-7A42-EB39-862B337F6601}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6626086" y="32487704"/>
+          <a:ext cx="2170295" cy="947530"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>86139</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>410816</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>775382</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1232452</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Picture 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{586DD17A-C5AA-0A7F-367A-BDC1C9DD50BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9031356" y="32388312"/>
+          <a:ext cx="1881938" cy="821636"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>92767</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>238540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>251793</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>974035</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="56" name="Picture 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE6BC47E-3DA9-9F36-78E4-8964C3BA7B04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2478158" y="34502036"/>
+          <a:ext cx="1351722" cy="735495"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>463826</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1088517</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="58" name="Picture 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDEE28F1-D9EE-F61F-D7A7-19ACFBED0E6C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4174435" y="34263497"/>
+          <a:ext cx="2252869" cy="1088516"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>26504</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1139685</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1484244</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>2095929</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="59" name="Picture 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B94188D-95BC-6333-7870-3953F5893FFB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4200939" y="35403181"/>
+          <a:ext cx="3246783" cy="956244"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>24848</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>381000</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="93" name="Picture 92"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4058478" y="32020565"/>
-          <a:ext cx="2343979" cy="381000"/>
+      <xdr:colOff>132521</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1192697</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>781878</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1722387</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="61" name="Picture 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ED7C8FA-4F2E-DCA3-F95E-EB3FD707FADA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7805530" y="35456193"/>
+          <a:ext cx="2438400" cy="529690"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>205408</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>437322</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1451113</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>967012</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="62" name="Picture 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96C4F6DE-6BB2-1726-8D34-5E603F48B437}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10694504" y="34700818"/>
+          <a:ext cx="2438400" cy="529690"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3149,33 +3698,39 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>218661</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>324679</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>563217</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>1085022</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="95" name="Picture 94"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6377609" y="32020565"/>
-          <a:ext cx="2302565" cy="1085022"/>
+      <xdr:colOff>585103</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>954157</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="74" name="Picture 73">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CBEF58B-B156-56E8-2653-8CE2C3F08B3E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7891670" y="34588175"/>
+          <a:ext cx="2155485" cy="629478"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3187,33 +3742,39 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>563217</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>1085022</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="96" name="Picture 95"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8696739" y="32020565"/>
-          <a:ext cx="2302565" cy="1085022"/>
+      <xdr:colOff>324677</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1298714</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1570382</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1828404</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="94" name="Picture 93">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEB723BD-9973-BB99-716E-EC91A6DB8044}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10813773" y="35562210"/>
+          <a:ext cx="2438400" cy="529690"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3521,16 +4082,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16:R16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="47" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AD14" sqref="AD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="69.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="69.900000000000006" customHeight="1"/>
+  <cols>
+    <col min="11" max="11" width="24.88671875" customWidth="1"/>
+    <col min="15" max="15" width="15" customWidth="1"/>
+    <col min="18" max="18" width="29.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="15" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3564,7 +4130,7 @@
       <c r="U1" s="2"/>
       <c r="V1" s="1"/>
     </row>
-    <row r="2" spans="1:22" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="69.900000000000006" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -3589,9 +4155,9 @@
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
     </row>
-    <row r="3" spans="1:22" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="69.900000000000006" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -3614,7 +4180,7 @@
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
     </row>
-    <row r="4" spans="1:22" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="69.900000000000006" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -3639,7 +4205,7 @@
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
     </row>
-    <row r="5" spans="1:22" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="69.900000000000006" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -3664,7 +4230,7 @@
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
     </row>
-    <row r="6" spans="1:22" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="200.1" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -3689,7 +4255,7 @@
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
     </row>
-    <row r="7" spans="1:22" ht="350.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="350.1" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -3714,7 +4280,7 @@
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
     </row>
-    <row r="8" spans="1:22" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="69.900000000000006" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -3739,7 +4305,7 @@
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
     </row>
-    <row r="9" spans="1:22" ht="249.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="249.9" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -3764,7 +4330,7 @@
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
     </row>
-    <row r="10" spans="1:22" ht="399.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="399.9" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -3789,9 +4355,9 @@
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
     </row>
-    <row r="11" spans="1:22" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="80.099999999999994" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -3814,7 +4380,7 @@
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
     </row>
-    <row r="12" spans="1:22" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="69.900000000000006" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -3839,7 +4405,7 @@
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
     </row>
-    <row r="13" spans="1:22" ht="189.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="189.9" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -3864,7 +4430,7 @@
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
     </row>
-    <row r="14" spans="1:22" ht="369.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="369.9" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
@@ -3889,7 +4455,7 @@
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
     </row>
-    <row r="15" spans="1:22" ht="249.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="249.9" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
@@ -3914,9 +4480,9 @@
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
     </row>
-    <row r="16" spans="1:22" ht="180" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="180" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -3924,7 +4490,9 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="H16" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -3939,9 +4507,9 @@
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
     </row>
-    <row r="17" spans="1:21" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="183.6" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -3964,9 +4532,9 @@
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
     </row>
-    <row r="18" spans="1:21" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="117.6" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -3991,6 +4559,90 @@
     </row>
   </sheetData>
   <mergeCells count="108">
+    <mergeCell ref="S17:U17"/>
+    <mergeCell ref="S18:U18"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="S14:U14"/>
+    <mergeCell ref="S15:U15"/>
+    <mergeCell ref="S16:U16"/>
+    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="P15:R15"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="S12:U12"/>
+    <mergeCell ref="L12:O12"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="L14:O14"/>
+    <mergeCell ref="L15:O15"/>
+    <mergeCell ref="L16:O16"/>
+    <mergeCell ref="L17:O17"/>
+    <mergeCell ref="L18:O18"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="P10:R10"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="P12:R12"/>
+    <mergeCell ref="S13:U13"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="S9:U9"/>
+    <mergeCell ref="S10:U10"/>
+    <mergeCell ref="S11:U11"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="L8:O8"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="L13:O13"/>
+    <mergeCell ref="L9:O9"/>
+    <mergeCell ref="L10:O10"/>
+    <mergeCell ref="L11:O11"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="H1:K1"/>
@@ -4015,90 +4667,6 @@
     <mergeCell ref="D3:G3"/>
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="L3:O3"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="L7:O7"/>
-    <mergeCell ref="L8:O8"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="L13:O13"/>
-    <mergeCell ref="L9:O9"/>
-    <mergeCell ref="L10:O10"/>
-    <mergeCell ref="L11:O11"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="P6:R6"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="S6:U6"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="P7:R7"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="P12:R12"/>
-    <mergeCell ref="S13:U13"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="S9:U9"/>
-    <mergeCell ref="S10:U10"/>
-    <mergeCell ref="S11:U11"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="S12:U12"/>
-    <mergeCell ref="L12:O12"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="L14:O14"/>
-    <mergeCell ref="L15:O15"/>
-    <mergeCell ref="L16:O16"/>
-    <mergeCell ref="L17:O17"/>
-    <mergeCell ref="L18:O18"/>
-    <mergeCell ref="S17:U17"/>
-    <mergeCell ref="S18:U18"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="S14:U14"/>
-    <mergeCell ref="S15:U15"/>
-    <mergeCell ref="S16:U16"/>
-    <mergeCell ref="P14:R14"/>
-    <mergeCell ref="P15:R15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>